<commit_message>
fixup for copyright mentions
</commit_message>
<xml_diff>
--- a/tools/scf_toolbox/mapping-cis-controls-v8-and-scf-2025.2.2.xlsx
+++ b/tools/scf_toolbox/mapping-cis-controls-v8-and-scf-2025.2.2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/scf_toolbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12D2E1D7-989E-4D43-B880-E97BFCDB34AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FB9C29-01E3-FA4E-BDC4-A6E269517F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="-28020" windowWidth="50880" windowHeight="27860" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="-28020" windowWidth="50880" windowHeight="27860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9020" uniqueCount="7530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9020" uniqueCount="7532">
   <si>
     <t>type</t>
   </si>
@@ -22940,6 +22940,12 @@
   </si>
   <si>
     <t>Mechanisms exist to routinely review the content on publicly accessible systems for sensitive/regulated data and remove such information, if discovered.</t>
+  </si>
+  <si>
+    <t>SCF - CC BY-ND 4.0</t>
+  </si>
+  <si>
+    <t>SCF</t>
   </si>
 </sst>
 </file>
@@ -23300,9 +23306,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -23365,7 +23376,7 @@
         <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>7530</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -23373,7 +23384,7 @@
         <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>7531</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -23394,6 +23405,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -23486,7 +23498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>